<commit_message>
unuploaded invalidated data csv files generate
</commit_message>
<xml_diff>
--- a/public/unupload_report/supervisorDownload.xlsx
+++ b/public/unupload_report/supervisorDownload.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Sr.</t>
   </si>
@@ -40,9 +40,6 @@
     <t>XYZ</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>1754787878</t>
   </si>
   <si>
@@ -62,6 +59,24 @@
   </si>
   <si>
     <t>abcde</t>
+  </si>
+  <si>
+    <t>APSIS</t>
+  </si>
+  <si>
+    <t>01754787878</t>
+  </si>
+  <si>
+    <t>sup2222</t>
+  </si>
+  <si>
+    <t>APEX</t>
+  </si>
+  <si>
+    <t>01754787879</t>
+  </si>
+  <si>
+    <t>sup1111</t>
   </si>
   <si>
     <t>XYZ11</t>
@@ -129,7 +144,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -168,23 +183,23 @@
       <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="0" t="n">
+        <v>788545455</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>9</v>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -192,25 +207,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>787885552</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>9</v>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -218,25 +233,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1112223788</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>9</v>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -244,25 +259,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1112223567</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>9</v>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -272,23 +287,23 @@
       <c r="B6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="0" t="n">
+        <v>788545455</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>9</v>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -296,25 +311,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>787885552</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>9</v>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -322,25 +337,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>788545455</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>9</v>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -348,25 +363,77 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>787885552</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="B10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>7885145455</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>7871885552</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="G11" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>9</v>
+      <c r="H11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>